<commit_message>
terminado - reporte diario y requerimientos
</commit_message>
<xml_diff>
--- a/data/Operaciones - Modelo Parte Diario.xlsx
+++ b/data/Operaciones - Modelo Parte Diario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Desktop\Python Projects\smont_y_aragon\operaciones_cl\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D91032F-7BA6-47AE-A9F4-B8CBAE17ABCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A60487-61B1-498A-B349-7458E52AF08C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PARTE DIARIO" sheetId="3" r:id="rId1"/>
@@ -2493,8 +2493,8 @@
   </sheetPr>
   <dimension ref="A1:AJ89"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="130" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="55" zoomScaleNormal="130" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16:M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4923,7 +4923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CB60C8F-FA64-460D-BD6C-57A24419024E}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>

</xml_diff>